<commit_message>
Update Custom Sequence Functions.xlsx
</commit_message>
<xml_diff>
--- a/Custom Sequence Functions/Custom Sequence Functions.xlsx
+++ b/Custom Sequence Functions/Custom Sequence Functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/profmc/Library/CloudStorage/Dropbox/Lambda-Update-Project/Lambda-Development/Custom Sequence Functions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1C1F93-6A8A-B04E-8989-01D40FAEFCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2012C31-2B8D-4194-8E38-2A8D2F83078B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1860" windowWidth="32620" windowHeight="16940" activeTab="3" xr2:uid="{EE143372-40E0-6A42-AC8E-55223BA24E9F}"/>
+    <workbookView xWindow="-60" yWindow="450" windowWidth="28185" windowHeight="14190" activeTab="3" xr2:uid="{EE143372-40E0-6A42-AC8E-55223BA24E9F}"/>
   </bookViews>
   <sheets>
     <sheet name="SPAN" sheetId="1" r:id="rId1"/>
@@ -66,8 +66,25 @@
 </metadata>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="12"/>
@@ -96,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +450,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="532" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -471,9 +489,9 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5703125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="4.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
@@ -596,9 +614,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
@@ -802,9 +820,9 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
@@ -1132,15 +1150,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75138C4-48E7-254A-B0F1-29CE7B124205}">
-  <dimension ref="B2:C17"/>
+  <dimension ref="B2:G107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G7" sqref="G7:G107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:7">
       <c r="B2" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B3)</f>
         <v>=SEQ_REPEAT(1,5,3,0)</v>
@@ -1150,7 +1168,7 @@
         <v>=SEQ_REPEAT(1,5,3,1)</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:7">
       <c r="B3" cm="1">
         <f t="array" ref="B3:B17">SEQ_REPEAT(1,5,3,0)</f>
         <v>1</v>
@@ -1159,24 +1177,42 @@
         <f t="array" ref="C3:C17">SEQ_REPEAT(1,5,3,1)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:3">
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:3">
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:3">
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
       <c r="B6">
         <v>2</v>
       </c>
@@ -1184,92 +1220,880 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:7">
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:3">
+      <c r="F7" cm="1">
+        <f t="array" ref="F7:F107">_xlfn.SEQUENCE(101,,0.5,(1.5-0.5)/100)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="1" cm="1">
+        <f t="array" ref="G7:G107">SEQ_SPAN(0.1, 1.05, 101)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:3">
+      <c r="F8">
+        <v>0.51</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.10950000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:3">
+      <c r="F9">
+        <v>0.52</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.11900000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="2:3">
+      <c r="F10">
+        <v>0.53</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.12850000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="2:3">
+      <c r="F11">
+        <v>0.54</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.13800000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="2:3">
+      <c r="F12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.14750000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
       <c r="B13">
         <v>4</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:3">
+      <c r="F13">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.15700000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="2:3">
+      <c r="F14">
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.16650000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
       <c r="B15">
         <v>5</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="2:3">
+      <c r="F15">
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.17600000000000007</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
       <c r="B16">
         <v>5</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:3">
+      <c r="F16">
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.18550000000000008</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
       <c r="B17">
         <v>5</v>
       </c>
       <c r="C17">
         <v>5</v>
+      </c>
+      <c r="F17">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.19500000000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="F18">
+        <v>0.6100000000000001</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.2045000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="F19">
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.21400000000000011</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="F20">
+        <v>0.63000000000000012</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.22350000000000012</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="F21">
+        <v>0.64000000000000012</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.23300000000000012</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="F22">
+        <v>0.65000000000000013</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.24250000000000013</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="F23">
+        <v>0.66000000000000014</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.25200000000000011</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="F24">
+        <v>0.67000000000000015</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.26150000000000012</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="F25">
+        <v>0.68000000000000016</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.27100000000000013</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="F26">
+        <v>0.69000000000000017</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.28050000000000014</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="F27">
+        <v>0.70000000000000018</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.29000000000000015</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="F28">
+        <v>0.71000000000000019</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.29950000000000015</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="F29">
+        <v>0.7200000000000002</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.30900000000000016</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="F30">
+        <v>0.7300000000000002</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.31850000000000017</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="F31">
+        <v>0.74000000000000021</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.32800000000000018</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="F32">
+        <v>0.75000000000000022</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.33750000000000019</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7">
+      <c r="F33">
+        <v>0.76000000000000023</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.3470000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7">
+      <c r="F34">
+        <v>0.77000000000000024</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.35650000000000021</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7">
+      <c r="F35">
+        <v>0.78000000000000025</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.36600000000000021</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7">
+      <c r="F36">
+        <v>0.79000000000000026</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.37550000000000022</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7">
+      <c r="F37">
+        <v>0.80000000000000027</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.38500000000000023</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7">
+      <c r="F38">
+        <v>0.81000000000000028</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.39450000000000024</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7">
+      <c r="F39">
+        <v>0.82000000000000028</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.40400000000000025</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7">
+      <c r="F40">
+        <v>0.83000000000000029</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.41350000000000026</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7">
+      <c r="F41">
+        <v>0.8400000000000003</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.42300000000000026</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7">
+      <c r="F42">
+        <v>0.85000000000000031</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0.43250000000000027</v>
+      </c>
+    </row>
+    <row r="43" spans="6:7">
+      <c r="F43">
+        <v>0.86000000000000032</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0.44200000000000028</v>
+      </c>
+    </row>
+    <row r="44" spans="6:7">
+      <c r="F44">
+        <v>0.87000000000000033</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0.45150000000000029</v>
+      </c>
+    </row>
+    <row r="45" spans="6:7">
+      <c r="F45">
+        <v>0.88000000000000034</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0.4610000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="6:7">
+      <c r="F46">
+        <v>0.89000000000000035</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.47050000000000031</v>
+      </c>
+    </row>
+    <row r="47" spans="6:7">
+      <c r="F47">
+        <v>0.90000000000000036</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.48000000000000032</v>
+      </c>
+    </row>
+    <row r="48" spans="6:7">
+      <c r="F48">
+        <v>0.91000000000000036</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.48950000000000032</v>
+      </c>
+    </row>
+    <row r="49" spans="6:7">
+      <c r="F49">
+        <v>0.92000000000000037</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0.49900000000000033</v>
+      </c>
+    </row>
+    <row r="50" spans="6:7">
+      <c r="F50">
+        <v>0.93000000000000038</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0.50850000000000029</v>
+      </c>
+    </row>
+    <row r="51" spans="6:7">
+      <c r="F51">
+        <v>0.94000000000000039</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0.51800000000000024</v>
+      </c>
+    </row>
+    <row r="52" spans="6:7">
+      <c r="F52">
+        <v>0.9500000000000004</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0.52750000000000019</v>
+      </c>
+    </row>
+    <row r="53" spans="6:7">
+      <c r="F53">
+        <v>0.96000000000000041</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0.53700000000000014</v>
+      </c>
+    </row>
+    <row r="54" spans="6:7">
+      <c r="F54">
+        <v>0.97000000000000042</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0.5465000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="6:7">
+      <c r="F55">
+        <v>0.98000000000000043</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="56" spans="6:7">
+      <c r="F56">
+        <v>0.99000000000000044</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0.5655</v>
+      </c>
+    </row>
+    <row r="57" spans="6:7">
+      <c r="F57">
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0.57499999999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="6:7">
+      <c r="F58">
+        <v>1.0100000000000005</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0.58449999999999991</v>
+      </c>
+    </row>
+    <row r="59" spans="6:7">
+      <c r="F59">
+        <v>1.0200000000000005</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0.59399999999999986</v>
+      </c>
+    </row>
+    <row r="60" spans="6:7">
+      <c r="F60">
+        <v>1.0300000000000005</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0.60349999999999981</v>
+      </c>
+    </row>
+    <row r="61" spans="6:7">
+      <c r="F61">
+        <v>1.0400000000000005</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0.61299999999999977</v>
+      </c>
+    </row>
+    <row r="62" spans="6:7">
+      <c r="F62">
+        <v>1.0500000000000005</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0.62249999999999972</v>
+      </c>
+    </row>
+    <row r="63" spans="6:7">
+      <c r="F63">
+        <v>1.0600000000000005</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0.63199999999999967</v>
+      </c>
+    </row>
+    <row r="64" spans="6:7">
+      <c r="F64">
+        <v>1.0700000000000005</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0.64149999999999963</v>
+      </c>
+    </row>
+    <row r="65" spans="6:7">
+      <c r="F65">
+        <v>1.0800000000000005</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0.65099999999999958</v>
+      </c>
+    </row>
+    <row r="66" spans="6:7">
+      <c r="F66">
+        <v>1.0900000000000005</v>
+      </c>
+      <c r="G66" s="1">
+        <v>0.66049999999999953</v>
+      </c>
+    </row>
+    <row r="67" spans="6:7">
+      <c r="F67">
+        <v>1.1000000000000005</v>
+      </c>
+      <c r="G67" s="1">
+        <v>0.66999999999999948</v>
+      </c>
+    </row>
+    <row r="68" spans="6:7">
+      <c r="F68">
+        <v>1.1100000000000005</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0.67949999999999944</v>
+      </c>
+    </row>
+    <row r="69" spans="6:7">
+      <c r="F69">
+        <v>1.1200000000000006</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0.68899999999999939</v>
+      </c>
+    </row>
+    <row r="70" spans="6:7">
+      <c r="F70">
+        <v>1.1300000000000006</v>
+      </c>
+      <c r="G70" s="1">
+        <v>0.69849999999999934</v>
+      </c>
+    </row>
+    <row r="71" spans="6:7">
+      <c r="F71">
+        <v>1.1400000000000006</v>
+      </c>
+      <c r="G71" s="1">
+        <v>0.7079999999999993</v>
+      </c>
+    </row>
+    <row r="72" spans="6:7">
+      <c r="F72">
+        <v>1.1500000000000006</v>
+      </c>
+      <c r="G72" s="1">
+        <v>0.71749999999999925</v>
+      </c>
+    </row>
+    <row r="73" spans="6:7">
+      <c r="F73">
+        <v>1.1600000000000006</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0.7269999999999992</v>
+      </c>
+    </row>
+    <row r="74" spans="6:7">
+      <c r="F74">
+        <v>1.1700000000000006</v>
+      </c>
+      <c r="G74" s="1">
+        <v>0.73649999999999916</v>
+      </c>
+    </row>
+    <row r="75" spans="6:7">
+      <c r="F75">
+        <v>1.1800000000000006</v>
+      </c>
+      <c r="G75" s="1">
+        <v>0.74599999999999911</v>
+      </c>
+    </row>
+    <row r="76" spans="6:7">
+      <c r="F76">
+        <v>1.1900000000000006</v>
+      </c>
+      <c r="G76" s="1">
+        <v>0.75549999999999906</v>
+      </c>
+    </row>
+    <row r="77" spans="6:7">
+      <c r="F77">
+        <v>1.2000000000000006</v>
+      </c>
+      <c r="G77" s="1">
+        <v>0.76499999999999901</v>
+      </c>
+    </row>
+    <row r="78" spans="6:7">
+      <c r="F78">
+        <v>1.2100000000000006</v>
+      </c>
+      <c r="G78" s="1">
+        <v>0.77449999999999897</v>
+      </c>
+    </row>
+    <row r="79" spans="6:7">
+      <c r="F79">
+        <v>1.2200000000000006</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0.78399999999999892</v>
+      </c>
+    </row>
+    <row r="80" spans="6:7">
+      <c r="F80">
+        <v>1.2300000000000006</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0.79349999999999887</v>
+      </c>
+    </row>
+    <row r="81" spans="6:7">
+      <c r="F81">
+        <v>1.2400000000000007</v>
+      </c>
+      <c r="G81" s="1">
+        <v>0.80299999999999883</v>
+      </c>
+    </row>
+    <row r="82" spans="6:7">
+      <c r="F82">
+        <v>1.2500000000000007</v>
+      </c>
+      <c r="G82" s="1">
+        <v>0.81249999999999878</v>
+      </c>
+    </row>
+    <row r="83" spans="6:7">
+      <c r="F83">
+        <v>1.2600000000000007</v>
+      </c>
+      <c r="G83" s="1">
+        <v>0.82199999999999873</v>
+      </c>
+    </row>
+    <row r="84" spans="6:7">
+      <c r="F84">
+        <v>1.2700000000000007</v>
+      </c>
+      <c r="G84" s="1">
+        <v>0.83149999999999868</v>
+      </c>
+    </row>
+    <row r="85" spans="6:7">
+      <c r="F85">
+        <v>1.2800000000000007</v>
+      </c>
+      <c r="G85" s="1">
+        <v>0.84099999999999864</v>
+      </c>
+    </row>
+    <row r="86" spans="6:7">
+      <c r="F86">
+        <v>1.2900000000000007</v>
+      </c>
+      <c r="G86" s="1">
+        <v>0.85049999999999859</v>
+      </c>
+    </row>
+    <row r="87" spans="6:7">
+      <c r="F87">
+        <v>1.3000000000000007</v>
+      </c>
+      <c r="G87" s="1">
+        <v>0.85999999999999854</v>
+      </c>
+    </row>
+    <row r="88" spans="6:7">
+      <c r="F88">
+        <v>1.3100000000000007</v>
+      </c>
+      <c r="G88" s="1">
+        <v>0.8694999999999985</v>
+      </c>
+    </row>
+    <row r="89" spans="6:7">
+      <c r="F89">
+        <v>1.3200000000000007</v>
+      </c>
+      <c r="G89" s="1">
+        <v>0.87899999999999845</v>
+      </c>
+    </row>
+    <row r="90" spans="6:7">
+      <c r="F90">
+        <v>1.3300000000000007</v>
+      </c>
+      <c r="G90" s="1">
+        <v>0.8884999999999984</v>
+      </c>
+    </row>
+    <row r="91" spans="6:7">
+      <c r="F91">
+        <v>1.3400000000000007</v>
+      </c>
+      <c r="G91" s="1">
+        <v>0.89799999999999836</v>
+      </c>
+    </row>
+    <row r="92" spans="6:7">
+      <c r="F92">
+        <v>1.3500000000000008</v>
+      </c>
+      <c r="G92" s="1">
+        <v>0.90749999999999831</v>
+      </c>
+    </row>
+    <row r="93" spans="6:7">
+      <c r="F93">
+        <v>1.3600000000000008</v>
+      </c>
+      <c r="G93" s="1">
+        <v>0.91699999999999826</v>
+      </c>
+    </row>
+    <row r="94" spans="6:7">
+      <c r="F94">
+        <v>1.3700000000000008</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0.92649999999999821</v>
+      </c>
+    </row>
+    <row r="95" spans="6:7">
+      <c r="F95">
+        <v>1.3800000000000008</v>
+      </c>
+      <c r="G95" s="1">
+        <v>0.93599999999999817</v>
+      </c>
+    </row>
+    <row r="96" spans="6:7">
+      <c r="F96">
+        <v>1.3900000000000008</v>
+      </c>
+      <c r="G96" s="1">
+        <v>0.94549999999999812</v>
+      </c>
+    </row>
+    <row r="97" spans="6:7">
+      <c r="F97">
+        <v>1.4000000000000008</v>
+      </c>
+      <c r="G97" s="1">
+        <v>0.95499999999999807</v>
+      </c>
+    </row>
+    <row r="98" spans="6:7">
+      <c r="F98">
+        <v>1.4100000000000008</v>
+      </c>
+      <c r="G98" s="1">
+        <v>0.96449999999999803</v>
+      </c>
+    </row>
+    <row r="99" spans="6:7">
+      <c r="F99">
+        <v>1.4200000000000008</v>
+      </c>
+      <c r="G99" s="1">
+        <v>0.97399999999999798</v>
+      </c>
+    </row>
+    <row r="100" spans="6:7">
+      <c r="F100">
+        <v>1.4300000000000008</v>
+      </c>
+      <c r="G100" s="1">
+        <v>0.98349999999999793</v>
+      </c>
+    </row>
+    <row r="101" spans="6:7">
+      <c r="F101">
+        <v>1.4400000000000008</v>
+      </c>
+      <c r="G101" s="1">
+        <v>0.99299999999999788</v>
+      </c>
+    </row>
+    <row r="102" spans="6:7">
+      <c r="F102">
+        <v>1.4500000000000008</v>
+      </c>
+      <c r="G102" s="1">
+        <v>1.0024999999999979</v>
+      </c>
+    </row>
+    <row r="103" spans="6:7">
+      <c r="F103">
+        <v>1.4600000000000009</v>
+      </c>
+      <c r="G103" s="1">
+        <v>1.011999999999998</v>
+      </c>
+    </row>
+    <row r="104" spans="6:7">
+      <c r="F104">
+        <v>1.4700000000000009</v>
+      </c>
+      <c r="G104" s="1">
+        <v>1.0214999999999981</v>
+      </c>
+    </row>
+    <row r="105" spans="6:7">
+      <c r="F105">
+        <v>1.4800000000000009</v>
+      </c>
+      <c r="G105" s="1">
+        <v>1.0309999999999981</v>
+      </c>
+    </row>
+    <row r="106" spans="6:7">
+      <c r="F106">
+        <v>1.4900000000000009</v>
+      </c>
+      <c r="G106" s="1">
+        <v>1.0404999999999982</v>
+      </c>
+    </row>
+    <row r="107" spans="6:7">
+      <c r="F107">
+        <v>1.5000000000000009</v>
+      </c>
+      <c r="G107" s="1">
+        <v>1.0499999999999983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>